<commit_message>
added eval results cutto
</commit_message>
<xml_diff>
--- a/tables/gmm_analysis/GMM Results.xlsx
+++ b/tables/gmm_analysis/GMM Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\MLPR\mlpr\tables\gmm_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6F0635-06DB-4339-949D-17C31A391CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70422B17-2BFF-407C-A34C-0B7C8A18D98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="177">
   <si>
     <t>Dataset</t>
   </si>
@@ -592,7 +592,8 @@
 ($2^5$ components, NO PCA, Z-Norm)</t>
   </si>
   <si>
-    <t>RBF SVM()</t>
+    <t>RBF SVM
+(PCA $m=5$, NO Z-Norm, $\gamma=10^{-3}, C=10,k=1$)</t>
   </si>
 </sst>
 </file>
@@ -603,7 +604,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,10 +746,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1130,7 +1169,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1162,41 +1201,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1243,7 +1333,359 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="106">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -2872,7 +3314,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C6659F82-CA48-4B51-AEC5-D400FF3F9408}" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C6659F82-CA48-4B51-AEC5-D400FF3F9408}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" showHeaders="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:I29" firstHeaderRow="1" firstDataRow="3" firstDataCol="3"/>
   <pivotFields count="7">
     <pivotField axis="axisCol" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -3036,50 +3478,50 @@
     <dataField name="Min of MinDCFParsed" fld="6" subtotal="min" baseField="1" baseItem="0"/>
   </dataFields>
   <formats count="14">
-    <format dxfId="43">
+    <format dxfId="99">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="98">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="97">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="96">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="93">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0" minSubtotal="1"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="92">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="91">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="90">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="89">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="88">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0" minSubtotal="1"/>
@@ -3119,12 +3561,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{445C10D1-E9CA-4F14-9F3A-5CC1054D1DF2}" name="Table_results" displayName="Table_results" ref="A1:G145" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G145" xr:uid="{445C10D1-E9CA-4F14-9F3A-5CC1054D1DF2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E1F6B4B8-FF9A-436C-B162-F52AED539A01}" uniqueName="1" name="# Prior" queryTableFieldId="1" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{826BF678-18F7-4C59-A1C3-9E15C08ED5A2}" uniqueName="4" name="Dataset" queryTableFieldId="4" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{E84CBD81-3D35-4E33-A3E9-37A01CF0DAA1}" uniqueName="2" name="MVG" queryTableFieldId="13" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{824C56C9-D83F-4FB6-AE8B-F6A066D596E4}" uniqueName="3" name="PCA" queryTableFieldId="3" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{235BF819-38E7-4BB0-88FA-7E857267187B}" uniqueName="5" name="Components" queryTableFieldId="14" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{031D9B45-EFA6-4BA0-B535-D799E4D3ED13}" uniqueName="7" name="MinDCF" queryTableFieldId="11" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{E1F6B4B8-FF9A-436C-B162-F52AED539A01}" uniqueName="1" name="# Prior" queryTableFieldId="1" dataDxfId="105"/>
+    <tableColumn id="4" xr3:uid="{826BF678-18F7-4C59-A1C3-9E15C08ED5A2}" uniqueName="4" name="Dataset" queryTableFieldId="4" dataDxfId="104"/>
+    <tableColumn id="2" xr3:uid="{E84CBD81-3D35-4E33-A3E9-37A01CF0DAA1}" uniqueName="2" name="MVG" queryTableFieldId="13" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{824C56C9-D83F-4FB6-AE8B-F6A066D596E4}" uniqueName="3" name="PCA" queryTableFieldId="3" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{235BF819-38E7-4BB0-88FA-7E857267187B}" uniqueName="5" name="Components" queryTableFieldId="14" dataDxfId="101"/>
+    <tableColumn id="7" xr3:uid="{031D9B45-EFA6-4BA0-B535-D799E4D3ED13}" uniqueName="7" name="MinDCF" queryTableFieldId="11" dataDxfId="100"/>
     <tableColumn id="6" xr3:uid="{632984EE-D1BC-447C-BCA5-768C8DCC9DA2}" uniqueName="6" name="MinDCFParsed" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7500,16 +7942,15 @@
   <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G11" sqref="A2:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
@@ -7525,90 +7966,90 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
     </row>
     <row r="2" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="15" t="s">
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="J2" s="15"/>
+      <c r="J2" s="31"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="5" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="35" t="s">
         <v>3</v>
       </c>
       <c r="O3" s="3"/>
@@ -7623,35 +8064,35 @@
       <c r="X3" s="3"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="36">
         <v>0.13400000000000001</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="36">
         <v>0.53</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="36">
         <v>0.17899999999999999</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="36">
         <v>0.13800000000000001</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="36">
         <v>0.53</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="36">
         <v>0.17799999999999999</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="37">
         <f t="shared" ref="I4:I15" si="0">AVERAGE(C4,D4)</f>
         <v>0.33200000000000002</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="37">
         <f t="shared" ref="J4:J15" si="1">AVERAGE(F4,G4)</f>
         <v>0.33400000000000002</v>
       </c>
@@ -7667,33 +8108,33 @@
       <c r="X4" s="3"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="36">
         <v>0.11700000000000001</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="36">
         <v>0.45</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="36">
         <v>0.19500000000000001</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="36">
         <v>0.129</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="36">
         <v>0.47099999999999997</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="36">
         <v>0.20499999999999999</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="37">
         <f t="shared" si="0"/>
         <v>0.28350000000000003</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="37">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
@@ -7713,33 +8154,33 @@
       <c r="X5" s="3"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="36">
         <v>0.11</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="36">
         <v>0.441</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="36">
         <v>0.183</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="36">
         <v>0.11700000000000001</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="36">
         <v>0.437</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="36">
         <v>0.17599999999999999</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="37">
         <f t="shared" si="0"/>
         <v>0.27550000000000002</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="37">
         <f t="shared" si="1"/>
         <v>0.27700000000000002</v>
       </c>
@@ -7759,293 +8200,293 @@
       <c r="X6" s="3"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="36">
         <v>0.10199999999999999</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="36">
         <v>0.42299999999999999</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="36">
         <v>0.17</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="36">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="36">
         <v>0.437</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="36">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="37">
         <f t="shared" si="0"/>
         <v>0.26250000000000001</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="37">
         <f t="shared" si="1"/>
         <v>0.26750000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="36">
         <v>0.123</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="36">
         <v>0.50600000000000001</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="36">
         <v>0.2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="36">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="36">
         <v>0.51100000000000001</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="36">
         <v>0.191</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="37">
         <f t="shared" si="0"/>
         <v>0.3145</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="37">
         <f t="shared" si="1"/>
         <v>0.32550000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="36">
         <v>0.14099999999999999</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="36">
         <v>0.51200000000000001</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="36">
         <v>0.251</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="36">
         <v>0.12</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="36">
         <v>0.497</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="36">
         <v>0.188</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="37">
         <f t="shared" si="0"/>
         <v>0.32650000000000001</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="37">
         <f t="shared" si="1"/>
         <v>0.3085</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="36">
         <v>0.14599999999999999</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="36">
         <v>0.47799999999999998</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="36">
         <v>0.22800000000000001</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="36">
         <v>0.11799999999999999</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="36">
         <v>0.504</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="36">
         <v>0.215</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="37">
         <f t="shared" si="0"/>
         <v>0.312</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="37">
         <f t="shared" si="1"/>
         <v>0.311</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A11" s="16"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="36">
         <v>0.16500000000000001</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="36">
         <v>0.51800000000000002</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="36">
         <v>0.23899999999999999</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="36">
         <v>0.13800000000000001</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="36">
         <v>0.48399999999999999</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="36">
         <v>0.23</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="37">
         <f t="shared" si="0"/>
         <v>0.34150000000000003</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="37">
         <f t="shared" si="1"/>
         <v>0.311</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="36">
         <v>0.121</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="36">
         <v>0.48899999999999999</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="36">
         <v>0.16600000000000001</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="36">
         <v>0.121</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="36">
         <v>0.48899999999999999</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="36">
         <v>0.16600000000000001</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="37">
         <f t="shared" si="0"/>
         <v>0.30499999999999999</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="37">
         <f t="shared" si="1"/>
         <v>0.30499999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="36">
         <v>0.115</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="36">
         <v>0.42899999999999999</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="36">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="36">
         <v>0.11899999999999999</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="36">
         <v>0.47799999999999998</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="36">
         <v>0.155</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="37">
         <f t="shared" si="0"/>
         <v>0.27200000000000002</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="37">
         <f t="shared" si="1"/>
         <v>0.29849999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="36">
         <v>0.121</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="36">
         <v>0.46300000000000002</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="36">
         <v>0.2</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="36">
         <v>0.11799999999999999</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="36">
         <v>0.46200000000000002</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="36">
         <v>0.20100000000000001</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="37">
         <f t="shared" si="0"/>
         <v>0.29200000000000004</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="37">
         <f t="shared" si="1"/>
         <v>0.29000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A15" s="16"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="36">
         <v>0.11</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="36">
         <v>0.51700000000000002</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="36">
         <v>0.21199999999999999</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="36">
         <v>0.112</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="36">
         <v>0.45700000000000002</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="36">
         <v>0.19400000000000001</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="37">
         <f t="shared" si="0"/>
         <v>0.3135</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="37">
         <f t="shared" si="1"/>
         <v>0.28450000000000003</v>
       </c>
@@ -8296,6 +8737,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="I1:P1"/>
     <mergeCell ref="Q1:X1"/>
@@ -8304,26 +8751,20 @@
     <mergeCell ref="U2:X2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:H27">
-    <cfRule type="top10" dxfId="29" priority="1" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="28" priority="2" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="27" priority="3" bottom="1" rank="3"/>
-    <cfRule type="top10" dxfId="26" priority="4" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="25" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="85" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="84" priority="2" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="83" priority="3" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="82" priority="4" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="81" priority="9" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J27">
-    <cfRule type="top10" dxfId="24" priority="5" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="23" priority="6" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="22" priority="7" bottom="1" rank="3"/>
-    <cfRule type="top10" dxfId="21" priority="8" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="20" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="80" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="79" priority="6" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="78" priority="7" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="77" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="76" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8361,59 +8802,59 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C1" s="4"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
     </row>
     <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
@@ -8435,10 +8876,10 @@
       <c r="Y3" s="3"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>169</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -8465,8 +8906,8 @@
       <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="2" t="s">
         <v>91</v>
       </c>
@@ -8493,8 +8934,8 @@
       <c r="Y5" s="3"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="2" t="s">
         <v>125</v>
       </c>
@@ -8521,8 +8962,8 @@
       <c r="Y6" s="3"/>
     </row>
     <row r="7" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="13" t="s">
         <v>167</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -8539,8 +8980,8 @@
       </c>
     </row>
     <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2" t="s">
         <v>91</v>
       </c>
@@ -8555,10 +8996,10 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>169</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -8575,8 +9016,8 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="2" t="s">
         <v>91</v>
       </c>
@@ -8591,8 +9032,8 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="2" t="s">
         <v>125</v>
       </c>
@@ -8607,8 +9048,8 @@
       </c>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="13" t="s">
         <v>167</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -8625,8 +9066,8 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="2" t="s">
         <v>91</v>
       </c>
@@ -8642,11 +9083,11 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
@@ -8669,10 +9110,10 @@
       <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>169</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -8694,8 +9135,8 @@
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="2" t="s">
         <v>91</v>
       </c>
@@ -8715,8 +9156,8 @@
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="15"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="2" t="s">
         <v>125</v>
       </c>
@@ -8736,8 +9177,8 @@
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="13" t="s">
         <v>167</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -8759,8 +9200,8 @@
       <c r="K19" s="10"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="15"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="2" t="s">
         <v>91</v>
       </c>
@@ -8780,10 +9221,10 @@
       <c r="K20" s="10"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>169</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -8805,8 +9246,8 @@
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="15"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="2" t="s">
         <v>91</v>
       </c>
@@ -8826,8 +9267,8 @@
       <c r="K22" s="10"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="15"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="2" t="s">
         <v>125</v>
       </c>
@@ -8847,8 +9288,8 @@
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="15"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="11"/>
+      <c r="B24" s="13" t="s">
         <v>167</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -8870,8 +9311,8 @@
       <c r="K24" s="10"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="15"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="2" t="s">
         <v>91</v>
       </c>
@@ -8893,10 +9334,10 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="11"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -8919,10 +9360,10 @@
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>169</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -8942,8 +9383,8 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="15"/>
-      <c r="B29" s="14"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="13"/>
       <c r="C29" s="2" t="s">
         <v>91</v>
       </c>
@@ -8961,8 +9402,8 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="15"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="2" t="s">
         <v>125</v>
       </c>
@@ -8980,8 +9421,8 @@
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="15"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="11"/>
+      <c r="B31" s="13" t="s">
         <v>167</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -9001,8 +9442,8 @@
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="15"/>
-      <c r="B32" s="14"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="2" t="s">
         <v>91</v>
       </c>
@@ -9020,10 +9461,10 @@
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>169</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -9043,8 +9484,8 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="15"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="2" t="s">
         <v>91</v>
       </c>
@@ -9062,8 +9503,8 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="15"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="2" t="s">
         <v>125</v>
       </c>
@@ -9081,8 +9522,8 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="15"/>
-      <c r="B36" s="14" t="s">
+      <c r="A36" s="11"/>
+      <c r="B36" s="13" t="s">
         <v>167</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -9102,8 +9543,8 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="15"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="13"/>
       <c r="C37" s="2" t="s">
         <v>91</v>
       </c>
@@ -9122,12 +9563,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="V2:Y2"/>
@@ -9138,33 +9586,26 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:Y1"/>
   </mergeCells>
   <conditionalFormatting sqref="D28:E37 J16:K27 L14:M15">
-    <cfRule type="top10" dxfId="19" priority="5" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="18" priority="6" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="17" priority="7" bottom="1" rank="3"/>
-    <cfRule type="top10" dxfId="16" priority="8" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="15" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="75" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="74" priority="6" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="73" priority="7" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="72" priority="8" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="71" priority="10" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:I27 D4:F13 D16:F25">
-    <cfRule type="top10" dxfId="14" priority="26" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="13" priority="27" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="12" priority="28" bottom="1" rank="3"/>
-    <cfRule type="top10" dxfId="11" priority="29" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="10" priority="30" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="70" priority="26" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="69" priority="27" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="68" priority="28" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="67" priority="29" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="66" priority="30" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9175,8 +9616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6E88E4-05DD-48AA-B159-AF77AE047C4F}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9188,56 +9629,57 @@
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="6.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C1" s="4"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
     </row>
     <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
@@ -9254,9 +9696,9 @@
       <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
@@ -9266,28 +9708,29 @@
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="N3" s="16"/>
+      <c r="O3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15" t="s">
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15" t="s">
+      <c r="R3" s="20"/>
+      <c r="S3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="19" t="s">
+      <c r="T3" s="20"/>
+      <c r="U3" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="V3" s="19"/>
+      <c r="V3" s="21"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
     </row>
     <row r="4" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -9305,28 +9748,29 @@
       <c r="F4" s="2">
         <v>0.2</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="N4" s="17"/>
+      <c r="O4" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="S4" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="T4" s="11" t="s">
+      <c r="T4" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="U4" s="11" t="s">
+      <c r="U4" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="V4" s="11" t="s">
+      <c r="V4" s="23" t="s">
         <v>172</v>
       </c>
       <c r="W4" s="3"/>
@@ -9334,7 +9778,7 @@
       <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="16"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="6" t="s">
         <v>167</v>
       </c>
@@ -9352,31 +9796,32 @@
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="24">
         <v>0.497</v>
       </c>
-      <c r="P5" s="21">
+      <c r="P5" s="25">
         <v>0.5464</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="24">
         <v>0.125</v>
       </c>
-      <c r="R5" s="21">
+      <c r="R5" s="25">
         <v>0.125</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5" s="24">
         <v>0.189</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="25">
         <v>0.189</v>
       </c>
-      <c r="U5" s="12">
+      <c r="U5" s="26">
+        <f>AVERAGE(O5,Q5)</f>
         <v>0.311</v>
       </c>
-      <c r="V5" s="3">
+      <c r="V5" s="24">
         <f>AVERAGE(P5,R5)</f>
         <v>0.3357</v>
       </c>
@@ -9384,8 +9829,8 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row r="6" spans="1:25" ht="87" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:25" ht="32" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -9405,40 +9850,41 @@
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="13" t="s">
+      <c r="N6" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="27">
         <v>0.37</v>
       </c>
-      <c r="P6" s="21">
+      <c r="P6" s="25">
         <v>0.4</v>
       </c>
-      <c r="Q6" s="12">
+      <c r="Q6" s="28">
         <v>0.106</v>
       </c>
-      <c r="R6" s="21">
+      <c r="R6" s="25">
         <v>0.108</v>
       </c>
-      <c r="S6" s="12">
+      <c r="S6" s="28">
         <v>0.152</v>
       </c>
-      <c r="T6" s="21">
+      <c r="T6" s="25">
         <v>0.16400000000000001</v>
       </c>
-      <c r="U6" s="12">
+      <c r="U6" s="26">
+        <f t="shared" ref="U6:U9" si="0">AVERAGE(O6,Q6)</f>
         <v>0.23799999999999999</v>
       </c>
-      <c r="V6" s="3">
-        <f t="shared" ref="V6:V8" si="0">AVERAGE(P6,R6)</f>
+      <c r="V6" s="24">
+        <f t="shared" ref="V6:V8" si="1">AVERAGE(P6,R6)</f>
         <v>0.254</v>
       </c>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
     </row>
-    <row r="7" spans="1:25" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
+    <row r="7" spans="1:25" ht="32" x14ac:dyDescent="0.35">
+      <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
         <v>167</v>
       </c>
@@ -9454,68 +9900,79 @@
       <c r="F7" s="2">
         <v>0.16400000000000001</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="28">
         <v>0.39100000000000001</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="P7" s="29">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="Q7" s="28">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="S7" s="12">
+      <c r="R7" s="29">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="S7" s="28">
         <v>0.159</v>
       </c>
-      <c r="U7" s="12">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="V7" s="3" t="e">
+      <c r="T7" s="29">
+        <v>0.187</v>
+      </c>
+      <c r="U7" s="26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+        <v>0.24149999999999999</v>
+      </c>
+      <c r="V7" s="24">
+        <f t="shared" si="1"/>
+        <v>0.4975</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="16" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="18"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="29">
         <v>0.109</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="29">
         <v>0.14399999999999999</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="29">
         <v>0.41199999999999998</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="29">
         <v>0.42299999999999999</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="29">
         <v>0.20399999999999999</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="29">
         <v>0.316</v>
       </c>
-      <c r="U8" s="12">
+      <c r="U8" s="26">
+        <f t="shared" si="0"/>
         <v>0.26050000000000001</v>
       </c>
-      <c r="V8" s="3">
-        <f t="shared" si="0"/>
+      <c r="V8" s="24">
+        <f t="shared" si="1"/>
         <v>0.28349999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" ht="24" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -9531,12 +9988,38 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="18" t="s">
         <v>176</v>
       </c>
+      <c r="O9" s="29">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="Q9" s="29">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="R9" s="29">
+        <v>0.154</v>
+      </c>
+      <c r="S9" s="29">
+        <v>0.186</v>
+      </c>
+      <c r="T9" s="29">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="U9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="V9" s="24">
+        <f>AVERAGE(P9,R9)</f>
+        <v>0.48599999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -9559,7 +10042,7 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="16"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="6" t="s">
         <v>167</v>
       </c>
@@ -9580,7 +10063,7 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -9601,9 +10084,26 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" s="20"/>
+      <c r="U12" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="V12" s="21"/>
     </row>
     <row r="13" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="16"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="6" t="s">
         <v>167</v>
       </c>
@@ -9622,21 +10122,75 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="N13" s="17"/>
+      <c r="O13" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q13" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="R13" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="S13" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="T13" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="V13" s="23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="16" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="N14" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="O14" s="24">
+        <v>0.497</v>
+      </c>
+      <c r="P14" s="25">
+        <v>0.5464</v>
+      </c>
+      <c r="Q14" s="24">
+        <v>0.125</v>
+      </c>
+      <c r="R14" s="25">
+        <v>0.125</v>
+      </c>
+      <c r="S14" s="24">
+        <v>0.189</v>
+      </c>
+      <c r="T14" s="25">
+        <v>0.189</v>
+      </c>
+      <c r="U14" s="26">
+        <f>AVERAGE(O14,Q14)</f>
+        <v>0.311</v>
+      </c>
+      <c r="V14" s="24">
+        <f>AVERAGE(P14,R14)</f>
+        <v>0.3357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="32" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -9650,9 +10204,38 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+      <c r="N15" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="O15" s="27">
+        <v>0.37</v>
+      </c>
+      <c r="P15" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="Q15" s="28">
+        <v>0.106</v>
+      </c>
+      <c r="R15" s="25">
+        <v>0.108</v>
+      </c>
+      <c r="S15" s="28">
+        <v>0.152</v>
+      </c>
+      <c r="T15" s="25">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="U15" s="26">
+        <f t="shared" ref="U15:U18" si="2">AVERAGE(O15,Q15)</f>
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="V15" s="24">
+        <f t="shared" ref="V15:V17" si="3">AVERAGE(P15,R15)</f>
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="32" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -9673,9 +10256,38 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
+      <c r="N16" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="O16" s="28">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="P16" s="29">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="Q16" s="28">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="R16" s="29">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="S16" s="28">
+        <v>0.159</v>
+      </c>
+      <c r="T16" s="29">
+        <v>0.187</v>
+      </c>
+      <c r="U16" s="26">
+        <f t="shared" si="2"/>
+        <v>0.24149999999999999</v>
+      </c>
+      <c r="V16" s="24">
+        <f t="shared" si="3"/>
+        <v>0.4975</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
         <v>167</v>
       </c>
@@ -9694,9 +10306,38 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="20" t="s">
+      <c r="N17" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="O17" s="29">
+        <v>0.109</v>
+      </c>
+      <c r="P17" s="29">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="Q17" s="29">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="R17" s="29">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="S17" s="29">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="T17" s="29">
+        <v>0.316</v>
+      </c>
+      <c r="U17" s="26">
+        <f t="shared" si="2"/>
+        <v>0.26050000000000001</v>
+      </c>
+      <c r="V17" s="24">
+        <f t="shared" si="3"/>
+        <v>0.28349999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -9717,9 +10358,38 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
+      <c r="N18" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="O18" s="29">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="P18" s="29">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="Q18" s="29">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="R18" s="29">
+        <v>0.154</v>
+      </c>
+      <c r="S18" s="29">
+        <v>0.186</v>
+      </c>
+      <c r="T18" s="29">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="U18" s="26">
+        <f t="shared" si="2"/>
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="V18" s="24">
+        <f>AVERAGE(P18,R18)</f>
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
         <v>167</v>
       </c>
@@ -9739,7 +10409,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="2"/>
@@ -9750,7 +10420,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="4"/>
       <c r="C21" s="2"/>
@@ -9761,7 +10431,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="2"/>
@@ -9772,7 +10442,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="4"/>
       <c r="C23" s="2"/>
@@ -9783,7 +10453,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="2"/>
@@ -9794,7 +10464,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="4"/>
       <c r="C25" s="2"/>
@@ -9805,7 +10475,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="2"/>
@@ -9816,7 +10486,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="4"/>
       <c r="C27" s="2"/>
@@ -9827,7 +10497,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C28" s="4"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -9837,7 +10507,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C29" s="4"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -9847,7 +10517,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C30" s="4"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -9857,7 +10527,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C31" s="4"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -9867,7 +10537,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C32" s="4"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -9928,13 +10598,9 @@
       <c r="J37" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="U3:V3"/>
+  <mergeCells count="24">
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="U12:V12"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="O3:P3"/>
@@ -9947,20 +10613,54 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="D14:E14"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="U3:V3"/>
   </mergeCells>
   <conditionalFormatting sqref="D16:E19">
-    <cfRule type="top10" dxfId="9" priority="5" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="8" priority="6" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="7" priority="7" bottom="1" rank="3"/>
-    <cfRule type="top10" dxfId="6" priority="8" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="5" priority="9" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="25" priority="21" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="22" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="23" priority="23" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="22" priority="24" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="21" priority="25" percent="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:F7 D10:F13">
-    <cfRule type="top10" dxfId="4" priority="1" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="3" priority="2" bottom="1" rank="2"/>
-    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="3"/>
-    <cfRule type="top10" dxfId="1" priority="4" percent="1" bottom="1" rank="10"/>
-    <cfRule type="top10" dxfId="0" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="20" priority="17" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="18" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="18" priority="19" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="17" priority="20" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="16" priority="26" percent="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:P9 R5:R9 T5:T9">
+    <cfRule type="top10" dxfId="13" priority="9" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="10" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="11" priority="14" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="10" priority="15" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="9" priority="16" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:V9">
+    <cfRule type="top10" dxfId="15" priority="11" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="12" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="8" priority="13" bottom="1" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14:P18 R14:R18 T14:T18">
+    <cfRule type="top10" dxfId="7" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="2" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="5" priority="6" bottom="1" rank="3"/>
+    <cfRule type="top10" dxfId="4" priority="7" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="8" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V14:V18">
+    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="4" bottom="1" rank="2"/>
+    <cfRule type="top10" dxfId="0" priority="5" bottom="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>